<commit_message>
Added an authentication filter (checks for logged in users and session highjacking). Changed the mapping of all servlets that require a logged in user (set them all to /auth/<servletName>). If the session is deemed invalid, the response is set with a code of 401. Must research how to handle the response code in the REST design.
</commit_message>
<xml_diff>
--- a/!Documentation/Tasks.xlsx
+++ b/!Documentation/Tasks.xlsx
@@ -15,8 +15,32 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="D21" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Should ask Krasi if it's implemented properly.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="44">
   <si>
     <t>Number</t>
   </si>
@@ -133,13 +157,28 @@
   </si>
   <si>
     <t>Rename all servlet mappings</t>
+  </si>
+  <si>
+    <t>Authentication filter</t>
+  </si>
+  <si>
+    <t>Finished ?</t>
+  </si>
+  <si>
+    <t>Added 1 filter for authenticating servlets that require a logged in user</t>
+  </si>
+  <si>
+    <t>Started</t>
+  </si>
+  <si>
+    <t>Filter sliders</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -156,8 +195,15 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -176,6 +222,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="17">
     <border>
@@ -423,7 +475,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -482,19 +534,28 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -822,7 +883,7 @@
   <dimension ref="A2:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -835,13 +896,13 @@
   <sheetData>
     <row r="2" spans="1:5" ht="15.75" thickBot="1"/>
     <row r="3" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" thickBot="1">
       <c r="A4" s="3" t="s">
@@ -912,19 +973,19 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="30">
-      <c r="A8" s="16">
+      <c r="A8" s="25">
         <v>4</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="7" t="s">
+      <c r="C8" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" s="27" t="s">
         <v>20</v>
       </c>
     </row>
@@ -963,19 +1024,19 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="45">
-      <c r="A11" s="18">
+      <c r="A11" s="25">
         <v>7</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="2" t="s">
+      <c r="D11" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="27" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1126,12 +1187,22 @@
       </c>
       <c r="E20" s="7"/>
     </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="18"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="2"/>
+    <row r="21" spans="1:5" ht="45">
+      <c r="A21" s="17">
+        <v>17</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="22" spans="1:5" ht="15.75" thickBot="1">
       <c r="A22" s="19"/>
@@ -1142,13 +1213,13 @@
     </row>
     <row r="23" spans="1:5" ht="15.75" thickBot="1"/>
     <row r="24" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A24" s="20" t="s">
+      <c r="A24" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="B24" s="20"/>
-      <c r="C24" s="20"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="20"/>
+      <c r="B24" s="24"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="24"/>
     </row>
     <row r="25" spans="1:5" ht="15.75" thickBot="1">
       <c r="A25" s="3" t="s">
@@ -1168,13 +1239,19 @@
       </c>
     </row>
     <row r="26" spans="1:5">
-      <c r="A26" s="21">
+      <c r="A26" s="20">
         <v>1</v>
       </c>
-      <c r="B26" s="22"/>
-      <c r="C26" s="23"/>
-      <c r="D26" s="22"/>
-      <c r="E26" s="24"/>
+      <c r="B26" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="C26" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="D26" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" s="23"/>
     </row>
     <row r="27" spans="1:5" ht="15.75" thickBot="1">
       <c r="A27" s="19">
@@ -1192,6 +1269,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added methods for creating new movies and tv series (added 1 new constructor for each with the full product information). Added 1 an example servlet for creating a movie and tested it (works with proper data). Have to reserach how to create JSON from form to remove parsing issues.
</commit_message>
<xml_diff>
--- a/!Documentation/Tasks.xlsx
+++ b/!Documentation/Tasks.xlsx
@@ -21,7 +21,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="D21" authorId="0">
+    <comment ref="D20" authorId="0">
       <text>
         <r>
           <rPr>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="45">
   <si>
     <t>Number</t>
   </si>
@@ -93,9 +93,6 @@
     <t>Editing Product Info</t>
   </si>
   <si>
-    <t>Putting Products On Promotion</t>
-  </si>
-  <si>
     <t>Not Assigned</t>
   </si>
   <si>
@@ -172,6 +169,12 @@
   </si>
   <si>
     <t>Filter sliders</t>
+  </si>
+  <si>
+    <t>Has Working Example</t>
+  </si>
+  <si>
+    <t>Have to read form as JSON data</t>
   </si>
 </sst>
 </file>
@@ -546,17 +549,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -880,10 +883,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:E27"/>
+  <dimension ref="A2:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -896,13 +899,13 @@
   <sheetData>
     <row r="2" spans="1:5" ht="15.75" thickBot="1"/>
     <row r="3" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A3" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
+      <c r="A3" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" thickBot="1">
       <c r="A4" s="3" t="s">
@@ -946,7 +949,7 @@
         <v>9</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>10</v>
@@ -973,20 +976,20 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="30">
-      <c r="A8" s="25">
+      <c r="A8" s="24">
         <v>4</v>
       </c>
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="26" t="s">
+      <c r="C8" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="E8" s="27" t="s">
-        <v>20</v>
+      <c r="D8" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" s="26" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="30">
@@ -997,274 +1000,257 @@
         <v>16</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E9" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="45">
+      <c r="A10" s="24">
+        <v>6</v>
+      </c>
+      <c r="B10" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" s="26" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="45">
+      <c r="A11" s="16">
+        <v>7</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="45">
-      <c r="A10" s="16">
-        <v>6</v>
-      </c>
-      <c r="B10" s="6" t="s">
+      <c r="C11" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="6" t="s">
+      <c r="D11" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="45">
-      <c r="A11" s="25">
+      <c r="E11" s="7"/>
+    </row>
+    <row r="12" spans="1:5" ht="60">
+      <c r="A12" s="18">
+        <v>8</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="45">
+      <c r="A13" s="16">
+        <v>9</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="120">
+      <c r="A14" s="18">
+        <v>10</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="60">
+      <c r="A15" s="16">
+        <v>11</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="30">
+      <c r="A16" s="18">
+        <v>12</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="45">
+      <c r="A17" s="16">
+        <v>13</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="60">
+      <c r="A18" s="18">
+        <v>14</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" spans="1:5" ht="45">
+      <c r="A19" s="16">
+        <v>15</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="7"/>
+    </row>
+    <row r="20" spans="1:5" ht="45">
+      <c r="A20" s="17">
+        <v>16</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A21" s="19"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="9"/>
+    </row>
+    <row r="22" spans="1:5" ht="15.75" thickBot="1"/>
+    <row r="23" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A23" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" s="27"/>
+      <c r="C23" s="27"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="27"/>
+    </row>
+    <row r="24" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A24" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E24" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="26" t="s">
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="20">
+        <v>1</v>
+      </c>
+      <c r="B25" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="E11" s="27" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="45">
-      <c r="A12" s="16">
-        <v>8</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" s="6" t="s">
+      <c r="C25" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="D25" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="7"/>
-    </row>
-    <row r="13" spans="1:5" ht="60">
-      <c r="A13" s="18">
-        <v>9</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="45">
-      <c r="A14" s="16">
-        <v>10</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="120">
-      <c r="A15" s="18">
-        <v>11</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="60">
-      <c r="A16" s="16">
-        <v>12</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="30">
-      <c r="A17" s="18">
-        <v>13</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="45">
-      <c r="A18" s="16">
-        <v>14</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="60">
-      <c r="A19" s="18">
-        <v>15</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E19" s="2"/>
-    </row>
-    <row r="20" spans="1:5" ht="45">
-      <c r="A20" s="16">
-        <v>16</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E20" s="7"/>
-    </row>
-    <row r="21" spans="1:5" ht="45">
-      <c r="A21" s="17">
-        <v>17</v>
-      </c>
-      <c r="B21" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="D21" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="E21" s="13" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A22" s="19"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="9"/>
-    </row>
-    <row r="23" spans="1:5" ht="15.75" thickBot="1"/>
-    <row r="24" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A24" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="B24" s="24"/>
-      <c r="C24" s="24"/>
-      <c r="D24" s="24"/>
-      <c r="E24" s="24"/>
-    </row>
-    <row r="25" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A25" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C25" s="4" t="s">
+      <c r="E25" s="23"/>
+    </row>
+    <row r="26" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A26" s="19">
         <v>2</v>
       </c>
-      <c r="D25" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="20">
-        <v>1</v>
-      </c>
-      <c r="B26" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="C26" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="D26" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="E26" s="23"/>
-    </row>
-    <row r="27" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A27" s="19">
-        <v>2</v>
-      </c>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="9"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A24:E24"/>
+    <mergeCell ref="A23:E23"/>
     <mergeCell ref="A3:E3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added some utility classes: 1) MailManager; 2) A custom TaskExecutor (used for executing daily tasks); 3) ExpiringProductsNotifier; Implemented the functionallity to notify users by email for all their products that are going to expire after 1 day. Fixed some select in the concrete DAO classes queries
</commit_message>
<xml_diff>
--- a/!Documentation/Tasks.xlsx
+++ b/!Documentation/Tasks.xlsx
@@ -108,9 +108,6 @@
     <t>Filtering products</t>
   </si>
   <si>
-    <t>Filter products by: year, price, genre, rating etc. (we have an example SQL built for this type of filtering)</t>
-  </si>
-  <si>
     <t>Product Ordering</t>
   </si>
   <si>
@@ -120,9 +117,6 @@
     <t>Notifications for products which are about to expire</t>
   </si>
   <si>
-    <t>Notifications for products that have expired???</t>
-  </si>
-  <si>
     <t>Same as 11 for expired products.</t>
   </si>
   <si>
@@ -175,6 +169,12 @@
   </si>
   <si>
     <t>Have to read form as JSON data</t>
+  </si>
+  <si>
+    <t>Filter products by: year, price, genre, rating etc. (The example SQL is in the GIT repository)</t>
+  </si>
+  <si>
+    <t>Removing expired products</t>
   </si>
 </sst>
 </file>
@@ -885,8 +885,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -900,7 +900,7 @@
     <row r="2" spans="1:5" ht="15.75" thickBot="1"/>
     <row r="3" spans="1:5" ht="15.75" thickBot="1">
       <c r="A3" s="27" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B3" s="27"/>
       <c r="C3" s="27"/>
@@ -986,10 +986,10 @@
         <v>13</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E8" s="26" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="30">
@@ -1020,10 +1020,10 @@
         <v>13</v>
       </c>
       <c r="D10" s="25" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E10" s="26" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="45">
@@ -1055,7 +1055,7 @@
         <v>10</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="45">
@@ -1063,7 +1063,7 @@
         <v>9</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>17</v>
@@ -1072,41 +1072,41 @@
         <v>10</v>
       </c>
       <c r="E13" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="120">
+      <c r="A14" s="17">
+        <v>10</v>
+      </c>
+      <c r="B14" s="12" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="120">
-      <c r="A14" s="18">
-        <v>10</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="60">
+      <c r="C14" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="45">
       <c r="A15" s="16">
         <v>11</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>10</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="30">
@@ -1114,7 +1114,7 @@
         <v>12</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>17</v>
@@ -1123,7 +1123,7 @@
         <v>10</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="45">
@@ -1131,7 +1131,7 @@
         <v>13</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>17</v>
@@ -1140,7 +1140,7 @@
         <v>10</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="60">
@@ -1148,7 +1148,7 @@
         <v>14</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>17</v>
@@ -1163,7 +1163,7 @@
         <v>15</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>17</v>
@@ -1178,16 +1178,16 @@
         <v>16</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C20" s="12" t="s">
         <v>13</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E20" s="13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="15.75" thickBot="1">
@@ -1200,7 +1200,7 @@
     <row r="22" spans="1:5" ht="15.75" thickBot="1"/>
     <row r="23" spans="1:5" ht="15.75" thickBot="1">
       <c r="A23" s="27" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B23" s="27"/>
       <c r="C23" s="27"/>
@@ -1229,7 +1229,7 @@
         <v>1</v>
       </c>
       <c r="B25" s="21" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C25" s="22" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
Implemented automatic deleteing of user's products if they are deemed expired. The custom executors get initiated as part of the main method of the utility WebSite class. Implemented (in last commit) closing of resources like executors and DB connections in the destroy method of the LoadupContextListener.
</commit_message>
<xml_diff>
--- a/!Documentation/Tasks.xlsx
+++ b/!Documentation/Tasks.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="44">
   <si>
     <t>Number</t>
   </si>
@@ -115,9 +115,6 @@
   </si>
   <si>
     <t>Notifications for products which are about to expire</t>
-  </si>
-  <si>
-    <t>Same as 11 for expired products.</t>
   </si>
   <si>
     <t>Sending emails to users that have 1 day left until some of their products expire. Group all expiring products in 1 email. (Can build a Map&lt;userId, List&lt;productId&gt;&gt; and create email message from there).</t>
@@ -886,7 +883,7 @@
   <dimension ref="A2:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -900,7 +897,7 @@
     <row r="2" spans="1:5" ht="15.75" thickBot="1"/>
     <row r="3" spans="1:5" ht="15.75" thickBot="1">
       <c r="A3" s="27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3" s="27"/>
       <c r="C3" s="27"/>
@@ -986,10 +983,10 @@
         <v>13</v>
       </c>
       <c r="D8" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="26" t="s">
         <v>41</v>
-      </c>
-      <c r="E8" s="26" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="30">
@@ -1020,10 +1017,10 @@
         <v>13</v>
       </c>
       <c r="D10" s="25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E10" s="26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="45">
@@ -1055,7 +1052,7 @@
         <v>10</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="45">
@@ -1089,32 +1086,30 @@
         <v>6</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="45">
-      <c r="A15" s="16">
+      <c r="A15" s="17">
         <v>11</v>
       </c>
-      <c r="B15" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C15" s="6" t="s">
+      <c r="B15" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>25</v>
-      </c>
+      <c r="D15" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="13"/>
     </row>
     <row r="16" spans="1:5" ht="30">
       <c r="A16" s="18">
         <v>12</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>17</v>
@@ -1123,7 +1118,7 @@
         <v>10</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="45">
@@ -1131,7 +1126,7 @@
         <v>13</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>17</v>
@@ -1140,7 +1135,7 @@
         <v>10</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="60">
@@ -1148,7 +1143,7 @@
         <v>14</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>17</v>
@@ -1163,7 +1158,7 @@
         <v>15</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>17</v>
@@ -1178,16 +1173,16 @@
         <v>16</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C20" s="12" t="s">
         <v>13</v>
       </c>
       <c r="D20" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="E20" s="13" t="s">
         <v>37</v>
-      </c>
-      <c r="E20" s="13" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="15.75" thickBot="1">
@@ -1200,7 +1195,7 @@
     <row r="22" spans="1:5" ht="15.75" thickBot="1"/>
     <row r="23" spans="1:5" ht="15.75" thickBot="1">
       <c r="A23" s="27" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B23" s="27"/>
       <c r="C23" s="27"/>
@@ -1229,7 +1224,7 @@
         <v>1</v>
       </c>
       <c r="B25" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C25" s="22" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
Added two new classes for dealing with queries for filtered products - ProductQueryInfo (holds the entire query parameters) and a JSON deserializer for that class. Implemented the method for filtering objects in the ProductDao (returns a list of product IDs). An example for it's work is added in the WebSite main method.
</commit_message>
<xml_diff>
--- a/!Documentation/Tasks.xlsx
+++ b/!Documentation/Tasks.xlsx
@@ -21,6 +21,20 @@
     <author>Author</author>
   </authors>
   <commentList>
+    <comment ref="E12" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Not implemented in a servlet. Otherwise successfully extracting filtered requests from JSON data.</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="D20" authorId="0">
       <text>
         <r>
@@ -882,8 +896,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1039,36 +1053,36 @@
       <c r="E11" s="7"/>
     </row>
     <row r="12" spans="1:5" ht="60">
-      <c r="A12" s="18">
+      <c r="A12" s="24">
         <v>8</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12" s="2" t="s">
+      <c r="C12" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="26" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="45">
-      <c r="A13" s="16">
+      <c r="A13" s="24">
         <v>9</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E13" s="7" t="s">
+      <c r="C13" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="26" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added a product categories table to the database schema and added it's POJO and DAO classes. Starting work on removing all caching logic (static collections) in the project.
</commit_message>
<xml_diff>
--- a/!Documentation/Tasks.xlsx
+++ b/!Documentation/Tasks.xlsx
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="48">
   <si>
     <t>Number</t>
   </si>
@@ -186,6 +186,18 @@
   </si>
   <si>
     <t>Removing expired products</t>
+  </si>
+  <si>
+    <t>Mario</t>
+  </si>
+  <si>
+    <t>Reviews</t>
+  </si>
+  <si>
+    <t>Implemented as DAO methods</t>
+  </si>
+  <si>
+    <t>Rate products</t>
   </si>
 </sst>
 </file>
@@ -217,7 +229,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -242,6 +254,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="17">
     <border>
@@ -489,7 +507,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -571,6 +589,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -896,8 +923,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -987,19 +1014,19 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="30">
-      <c r="A8" s="24">
+      <c r="A8" s="28">
         <v>4</v>
       </c>
-      <c r="B8" s="25" t="s">
+      <c r="B8" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="25" t="s">
+      <c r="C8" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="25" t="s">
+      <c r="D8" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="E8" s="26" t="s">
+      <c r="E8" s="30" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1038,51 +1065,53 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="45">
-      <c r="A11" s="16">
+      <c r="A11" s="28">
         <v>7</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="7"/>
+      <c r="C11" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="30" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="12" spans="1:5" ht="60">
-      <c r="A12" s="24">
+      <c r="A12" s="28">
         <v>8</v>
       </c>
-      <c r="B12" s="25" t="s">
+      <c r="B12" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="25" t="s">
+      <c r="C12" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="E12" s="26" t="s">
+      <c r="D12" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="30" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="45">
-      <c r="A13" s="24">
+      <c r="A13" s="28">
         <v>9</v>
       </c>
-      <c r="B13" s="25" t="s">
+      <c r="B13" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="25" t="s">
+      <c r="C13" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="E13" s="26" t="s">
+      <c r="D13" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="30" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1200,10 +1229,18 @@
       </c>
     </row>
     <row r="21" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A21" s="19"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
+      <c r="A21" s="19">
+        <v>17</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="E21" s="9"/>
     </row>
     <row r="22" spans="1:5" ht="15.75" thickBot="1"/>
@@ -1252,9 +1289,15 @@
       <c r="A26" s="19">
         <v>2</v>
       </c>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
+      <c r="B26" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="E26" s="9"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implemented Krasi's PictureServlet and tested it with the current main page. For it to work you need to create a folder in C:\images.
</commit_message>
<xml_diff>
--- a/!Documentation/Tasks.xlsx
+++ b/!Documentation/Tasks.xlsx
@@ -587,17 +587,17 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -923,8 +923,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -937,13 +937,13 @@
   <sheetData>
     <row r="2" spans="1:5" ht="15.75" thickBot="1"/>
     <row r="3" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" thickBot="1">
       <c r="A4" s="3" t="s">
@@ -1014,19 +1014,19 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="30">
-      <c r="A8" s="28">
+      <c r="A8" s="27">
         <v>4</v>
       </c>
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="29" t="s">
+      <c r="C8" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="29" t="s">
+      <c r="D8" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="E8" s="30" t="s">
+      <c r="E8" s="29" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1065,53 +1065,53 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="45">
-      <c r="A11" s="28">
+      <c r="A11" s="27">
         <v>7</v>
       </c>
-      <c r="B11" s="29" t="s">
+      <c r="B11" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="29" t="s">
+      <c r="C11" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="D11" s="29" t="s">
+      <c r="D11" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="30" t="s">
+      <c r="E11" s="29" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="60">
-      <c r="A12" s="28">
+      <c r="A12" s="27">
         <v>8</v>
       </c>
-      <c r="B12" s="29" t="s">
+      <c r="B12" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="29" t="s">
+      <c r="C12" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="29" t="s">
+      <c r="D12" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="30" t="s">
+      <c r="E12" s="29" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="45">
-      <c r="A13" s="28">
+      <c r="A13" s="27">
         <v>9</v>
       </c>
-      <c r="B13" s="29" t="s">
+      <c r="B13" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="29" t="s">
+      <c r="C13" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="29" t="s">
+      <c r="D13" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E13" s="30" t="s">
+      <c r="E13" s="29" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1245,13 +1245,13 @@
     </row>
     <row r="22" spans="1:5" ht="15.75" thickBot="1"/>
     <row r="23" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A23" s="27" t="s">
+      <c r="A23" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="B23" s="27"/>
-      <c r="C23" s="27"/>
-      <c r="D23" s="27"/>
-      <c r="E23" s="27"/>
+      <c r="B23" s="30"/>
+      <c r="C23" s="30"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="30"/>
     </row>
     <row r="24" spans="1:5" ht="15.75" thickBot="1">
       <c r="A24" s="3" t="s">

</xml_diff>